<commit_message>
Finished PS5 - Granger Causality
</commit_message>
<xml_diff>
--- a/Assignment 4-5/PS4_Data.xlsx
+++ b/Assignment 4-5/PS4_Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Evan\Documents\Umass\Econ 753\EvanWasner_Econ753_ProblemSets\Assignment 4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Evan\Documents\Umass\Econ 753\EvanWasner_Econ753_ProblemSets\Assignment 4-5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{772C786D-7C45-44D7-A42A-7279AED7FD9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A6219AB-4DE6-4946-A1E0-32C1669B1C80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ACB4FD60-BD01-4E4C-8D05-A38B29A15763}"/>
   </bookViews>
@@ -412,7 +412,7 @@
   <dimension ref="A1:H71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,8 +420,9 @@
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" customWidth="1"/>
+    <col min="6" max="6" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -467,8 +468,8 @@
         <v>-8318</v>
       </c>
       <c r="F2">
-        <f>D2+E2</f>
-        <v>8466</v>
+        <f>D2-E2</f>
+        <v>25102</v>
       </c>
       <c r="G2">
         <f>B2/C2</f>
@@ -476,7 +477,7 @@
       </c>
       <c r="H2">
         <f>F2/C2</f>
-        <v>0.44713214323439315</v>
+        <v>1.3257631773529102</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -496,8 +497,8 @@
         <v>-25717</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F66" si="0">D3+E3</f>
-        <v>-17690</v>
+        <f t="shared" ref="F3:F66" si="0">D3-E3</f>
+        <v>33744</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G66" si="1">B3/C3</f>
@@ -505,7 +506,7 @@
       </c>
       <c r="H3">
         <f t="shared" ref="H3:H66" si="2">F3/C3</f>
-        <v>-0.77765078248637243</v>
+        <v>1.4833831545630385</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -526,7 +527,7 @@
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>7048</v>
+        <v>3788</v>
       </c>
       <c r="G4">
         <f t="shared" si="1"/>
@@ -534,7 +535,7 @@
       </c>
       <c r="H4">
         <f t="shared" si="2"/>
-        <v>0.28937428149121364</v>
+        <v>0.15552635900804729</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -555,7 +556,7 @@
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>3753</v>
+        <v>2321</v>
       </c>
       <c r="G5">
         <f t="shared" si="1"/>
@@ -563,7 +564,7 @@
       </c>
       <c r="H5">
         <f t="shared" si="2"/>
-        <v>0.13965170797052914</v>
+        <v>8.6366004316439676E-2</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -584,7 +585,7 @@
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>-42938</v>
+        <v>53934</v>
       </c>
       <c r="G6">
         <f t="shared" si="1"/>
@@ -592,7 +593,7 @@
       </c>
       <c r="H6">
         <f t="shared" si="2"/>
-        <v>-1.6132401562969643</v>
+        <v>2.0263751127141569</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -613,7 +614,7 @@
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>-36618</v>
+        <v>71382</v>
       </c>
       <c r="G7">
         <f t="shared" si="1"/>
@@ -621,7 +622,7 @@
       </c>
       <c r="H7">
         <f t="shared" si="2"/>
-        <v>-1.2485253503358451</v>
+        <v>2.433836816802482</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -642,7 +643,7 @@
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>-26316</v>
+        <v>36378</v>
       </c>
       <c r="G8">
         <f t="shared" si="1"/>
@@ -650,7 +651,7 @@
       </c>
       <c r="H8">
         <f t="shared" si="2"/>
-        <v>-0.73888140161725069</v>
+        <v>1.0213948787061995</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -671,7 +672,7 @@
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>22382</v>
+        <v>-13260</v>
       </c>
       <c r="G9">
         <f t="shared" si="1"/>
@@ -679,7 +680,7 @@
       </c>
       <c r="H9">
         <f t="shared" si="2"/>
-        <v>0.58110914944438674</v>
+        <v>-0.34427251012566207</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -700,7 +701,7 @@
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>-65397</v>
+        <v>88457</v>
       </c>
       <c r="G10">
         <f t="shared" si="1"/>
@@ -708,7 +709,7 @@
       </c>
       <c r="H10">
         <f t="shared" si="2"/>
-        <v>-1.942350530161276</v>
+        <v>2.6272535566841904</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -729,7 +730,7 @@
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>-24047</v>
+        <v>54245</v>
       </c>
       <c r="G11">
         <f t="shared" si="1"/>
@@ -737,7 +738,7 @@
       </c>
       <c r="H11">
         <f t="shared" si="2"/>
-        <v>-0.64652901005538532</v>
+        <v>1.4584341560466743</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -758,7 +759,7 @@
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>-7745</v>
+        <v>13425</v>
       </c>
       <c r="G12">
         <f t="shared" si="1"/>
@@ -766,7 +767,7 @@
       </c>
       <c r="H12">
         <f t="shared" si="2"/>
-        <v>-0.1914756854310366</v>
+        <v>0.33189942891047985</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -787,7 +788,7 @@
       </c>
       <c r="F13">
         <f t="shared" si="0"/>
-        <v>-58340</v>
+        <v>85044</v>
       </c>
       <c r="G13">
         <f t="shared" si="1"/>
@@ -795,7 +796,7 @@
       </c>
       <c r="H13">
         <f t="shared" si="2"/>
-        <v>-1.4415260309851499</v>
+        <v>2.1013565268958021</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -816,7 +817,7 @@
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
-        <v>8303</v>
+        <v>15637</v>
       </c>
       <c r="G14">
         <f t="shared" si="1"/>
@@ -824,7 +825,7 @@
       </c>
       <c r="H14">
         <f t="shared" si="2"/>
-        <v>0.19033101045296166</v>
+        <v>0.3584494773519164</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -845,7 +846,7 @@
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
-        <v>3895</v>
+        <v>20137</v>
       </c>
       <c r="G15">
         <f t="shared" si="1"/>
@@ -853,7 +854,7 @@
       </c>
       <c r="H15">
         <f t="shared" si="2"/>
-        <v>8.384097122069871E-2</v>
+        <v>0.43345459241879586</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -874,7 +875,7 @@
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
-        <v>2441</v>
+        <v>23309</v>
       </c>
       <c r="G16">
         <f t="shared" si="1"/>
@@ -882,7 +883,7 @@
       </c>
       <c r="H16">
         <f t="shared" si="2"/>
-        <v>4.7064494360358623E-2</v>
+        <v>0.44941675503711559</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -903,7 +904,7 @@
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
-        <v>17066</v>
+        <v>35162</v>
       </c>
       <c r="G17">
         <f t="shared" si="1"/>
@@ -911,7 +912,7 @@
       </c>
       <c r="H17">
         <f t="shared" si="2"/>
-        <v>0.27658298624053934</v>
+        <v>0.56985883992674591</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -932,7 +933,7 @@
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
-        <v>-2227</v>
+        <v>35221</v>
       </c>
       <c r="G18">
         <f t="shared" si="1"/>
@@ -940,7 +941,7 @@
       </c>
       <c r="H18">
         <f t="shared" si="2"/>
-        <v>-3.0949039009408395E-2</v>
+        <v>0.48947287963644953</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -961,7 +962,7 @@
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
-        <v>-1605</v>
+        <v>30239</v>
       </c>
       <c r="G19">
         <f t="shared" si="1"/>
@@ -969,7 +970,7 @@
       </c>
       <c r="H19">
         <f t="shared" si="2"/>
-        <v>-2.1734125963140005E-2</v>
+        <v>0.40948176635476052</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -990,7 +991,7 @@
       </c>
       <c r="F20">
         <f t="shared" si="0"/>
-        <v>13951</v>
+        <v>48817</v>
       </c>
       <c r="G20">
         <f t="shared" si="1"/>
@@ -998,7 +999,7 @@
       </c>
       <c r="H20">
         <f t="shared" si="2"/>
-        <v>0.17378360198310869</v>
+        <v>0.60809935474227061</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1019,7 +1020,7 @@
       </c>
       <c r="F21">
         <f t="shared" si="0"/>
-        <v>16940</v>
+        <v>57824</v>
       </c>
       <c r="G21">
         <f t="shared" si="1"/>
@@ -1027,7 +1028,7 @@
       </c>
       <c r="H21">
         <f t="shared" si="2"/>
-        <v>0.1898145554372794</v>
+        <v>0.6479242534595776</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1048,7 +1049,7 @@
       </c>
       <c r="F22">
         <f t="shared" si="0"/>
-        <v>-2682</v>
+        <v>44908</v>
       </c>
       <c r="G22">
         <f t="shared" si="1"/>
@@ -1056,7 +1057,7 @@
       </c>
       <c r="H22">
         <f t="shared" si="2"/>
-        <v>-2.9056791835496521E-2</v>
+        <v>0.48653333622240036</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1077,7 +1078,7 @@
       </c>
       <c r="F23">
         <f t="shared" si="0"/>
-        <v>18738</v>
+        <v>57122</v>
       </c>
       <c r="G23">
         <f t="shared" si="1"/>
@@ -1085,7 +1086,7 @@
       </c>
       <c r="H23">
         <f t="shared" si="2"/>
-        <v>0.19646039967288054</v>
+        <v>0.59890121411646291</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1106,7 +1107,7 @@
       </c>
       <c r="F24">
         <f t="shared" si="0"/>
-        <v>50417</v>
+        <v>75151</v>
       </c>
       <c r="G24">
         <f t="shared" si="1"/>
@@ -1114,7 +1115,7 @@
       </c>
       <c r="H24">
         <f t="shared" si="2"/>
-        <v>0.46679814084402721</v>
+        <v>0.69580393681832486</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1135,7 +1136,7 @@
       </c>
       <c r="F25">
         <f t="shared" si="0"/>
-        <v>53358</v>
+        <v>119098</v>
       </c>
       <c r="G25">
         <f t="shared" si="1"/>
@@ -1143,7 +1144,7 @@
       </c>
       <c r="H25">
         <f t="shared" si="2"/>
-        <v>0.42367457777848355</v>
+        <v>0.94566503362685705</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1164,7 +1165,7 @@
       </c>
       <c r="F26">
         <f t="shared" si="0"/>
-        <v>34506</v>
+        <v>100074</v>
       </c>
       <c r="G26">
         <f t="shared" si="1"/>
@@ -1172,7 +1173,7 @@
       </c>
       <c r="H26">
         <f t="shared" si="2"/>
-        <v>0.24361246231723419</v>
+        <v>0.70652273673954946</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1193,7 +1194,7 @@
       </c>
       <c r="F27">
         <f t="shared" si="0"/>
-        <v>-12407</v>
+        <v>69961</v>
       </c>
       <c r="G27">
         <f t="shared" si="1"/>
@@ -1201,7 +1202,7 @@
       </c>
       <c r="H27">
         <f t="shared" si="2"/>
-        <v>-8.5976425260035891E-2</v>
+        <v>0.48480669683383343</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1222,7 +1223,7 @@
       </c>
       <c r="F28">
         <f t="shared" si="0"/>
-        <v>43270</v>
+        <v>112896</v>
       </c>
       <c r="G28">
         <f t="shared" si="1"/>
@@ -1230,7 +1231,7 @@
       </c>
       <c r="H28">
         <f t="shared" si="2"/>
-        <v>0.26703942333802366</v>
+        <v>0.69673405909797825</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -1251,7 +1252,7 @@
       </c>
       <c r="F29">
         <f t="shared" si="0"/>
-        <v>69615</v>
+        <v>148749</v>
       </c>
       <c r="G29">
         <f t="shared" si="1"/>
@@ -1259,7 +1260,7 @@
       </c>
       <c r="H29">
         <f t="shared" si="2"/>
-        <v>0.35944236478636893</v>
+        <v>0.76803407770749965</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -1280,7 +1281,7 @@
       </c>
       <c r="F30">
         <f t="shared" si="0"/>
-        <v>71012</v>
+        <v>196832</v>
       </c>
       <c r="G30">
         <f t="shared" si="1"/>
@@ -1288,7 +1289,7 @@
       </c>
       <c r="H30">
         <f t="shared" si="2"/>
-        <v>0.30341432984537031</v>
+        <v>0.84100784898501557</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -1309,7 +1310,7 @@
       </c>
       <c r="F31">
         <f t="shared" si="0"/>
-        <v>90113</v>
+        <v>249237</v>
       </c>
       <c r="G31">
         <f t="shared" si="1"/>
@@ -1317,7 +1318,7 @@
       </c>
       <c r="H31">
         <f t="shared" si="2"/>
-        <v>0.32718750113464312</v>
+        <v>0.90494413925066353</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -1338,7 +1339,7 @@
       </c>
       <c r="F32">
         <f t="shared" si="0"/>
-        <v>56334</v>
+        <v>232230</v>
       </c>
       <c r="G32">
         <f t="shared" si="1"/>
@@ -1346,7 +1347,7 @@
       </c>
       <c r="H32">
         <f t="shared" si="2"/>
-        <v>0.1872619087192102</v>
+        <v>0.77196423229066247</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -1367,7 +1368,7 @@
       </c>
       <c r="F33">
         <f t="shared" si="0"/>
-        <v>141121</v>
+        <v>268865</v>
       </c>
       <c r="G33">
         <f t="shared" si="1"/>
@@ -1375,7 +1376,7 @@
       </c>
       <c r="H33">
         <f t="shared" si="2"/>
-        <v>0.41019611490758157</v>
+        <v>0.78150933195362071</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -1396,7 +1397,7 @@
       </c>
       <c r="F34">
         <f t="shared" si="0"/>
-        <v>21198</v>
+        <v>166158</v>
       </c>
       <c r="G34">
         <f t="shared" si="1"/>
@@ -1404,7 +1405,7 @@
       </c>
       <c r="H34">
         <f t="shared" si="2"/>
-        <v>6.0363582517968403E-2</v>
+        <v>0.47315275705352361</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -1425,7 +1426,7 @@
       </c>
       <c r="F35">
         <f t="shared" si="0"/>
-        <v>128705</v>
+        <v>181405</v>
       </c>
       <c r="G35">
         <f t="shared" si="1"/>
@@ -1433,7 +1434,7 @@
       </c>
       <c r="H35">
         <f t="shared" si="2"/>
-        <v>0.36840222120448823</v>
+        <v>0.51924948477215482</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -1454,7 +1455,7 @@
       </c>
       <c r="F36">
         <f t="shared" si="0"/>
-        <v>289826</v>
+        <v>253554</v>
       </c>
       <c r="G36">
         <f t="shared" si="1"/>
@@ -1462,7 +1463,7 @@
       </c>
       <c r="H36">
         <f t="shared" si="2"/>
-        <v>0.71223969212772964</v>
+        <v>0.62310221614953232</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
@@ -1483,7 +1484,7 @@
       </c>
       <c r="F37">
         <f t="shared" si="0"/>
-        <v>142662</v>
+        <v>307082</v>
       </c>
       <c r="G37">
         <f t="shared" si="1"/>
@@ -1491,7 +1492,7 @@
       </c>
       <c r="H37">
         <f t="shared" si="2"/>
-        <v>0.32976817617593551</v>
+        <v>0.70983072630734634</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -1512,7 +1513,7 @@
       </c>
       <c r="F38">
         <f t="shared" si="0"/>
-        <v>138945</v>
+        <v>133757</v>
       </c>
       <c r="G38">
         <f t="shared" si="1"/>
@@ -1520,7 +1521,7 @@
       </c>
       <c r="H38">
         <f t="shared" si="2"/>
-        <v>0.32474179819241206</v>
+        <v>0.31261642161159064</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -1541,7 +1542,7 @@
       </c>
       <c r="F39">
         <f t="shared" si="0"/>
-        <v>208301</v>
+        <v>244589</v>
       </c>
       <c r="G39">
         <f t="shared" si="1"/>
@@ -1549,7 +1550,7 @@
       </c>
       <c r="H39">
         <f t="shared" si="2"/>
-        <v>0.49201396434274053</v>
+        <v>0.57772744021692912</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -1570,7 +1571,7 @@
       </c>
       <c r="F40">
         <f t="shared" si="0"/>
-        <v>352196</v>
+        <v>341646</v>
       </c>
       <c r="G40">
         <f t="shared" si="1"/>
@@ -1578,7 +1579,7 @@
       </c>
       <c r="H40">
         <f t="shared" si="2"/>
-        <v>0.7818828450025086</v>
+        <v>0.75846161360074238</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -1599,7 +1600,7 @@
       </c>
       <c r="F41">
         <f t="shared" si="0"/>
-        <v>77102</v>
+        <v>250620</v>
       </c>
       <c r="G41">
         <f t="shared" si="1"/>
@@ -1607,7 +1608,7 @@
       </c>
       <c r="H41">
         <f t="shared" si="2"/>
-        <v>0.15745513359854271</v>
+        <v>0.51180780761156353</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -1628,7 +1629,7 @@
       </c>
       <c r="F42">
         <f t="shared" si="0"/>
-        <v>59886</v>
+        <v>197200</v>
       </c>
       <c r="G42">
         <f t="shared" si="1"/>
@@ -1636,7 +1637,7 @@
       </c>
       <c r="H42">
         <f t="shared" si="2"/>
-        <v>0.11411769637977491</v>
+        <v>0.37578081231158555</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -1657,7 +1658,7 @@
       </c>
       <c r="F43">
         <f t="shared" si="0"/>
-        <v>-12316</v>
+        <v>115572</v>
       </c>
       <c r="G43">
         <f t="shared" si="1"/>
@@ -1665,7 +1666,7 @@
       </c>
       <c r="H43">
         <f t="shared" si="2"/>
-        <v>-2.3562813762703562E-2</v>
+        <v>0.22111087302559079</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -1686,7 +1687,7 @@
       </c>
       <c r="F44">
         <f t="shared" si="0"/>
-        <v>-32293</v>
+        <v>330347</v>
       </c>
       <c r="G44">
         <f t="shared" si="1"/>
@@ -1694,7 +1695,7 @@
       </c>
       <c r="H44">
         <f t="shared" si="2"/>
-        <v>-5.9687340583621053E-2</v>
+        <v>0.61058229027273603</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
@@ -1715,7 +1716,7 @@
       </c>
       <c r="F45">
         <f t="shared" si="0"/>
-        <v>354417</v>
+        <v>292099</v>
       </c>
       <c r="G45">
         <f t="shared" si="1"/>
@@ -1723,7 +1724,7 @@
       </c>
       <c r="H45">
         <f t="shared" si="2"/>
-        <v>0.6133532928950306</v>
+        <v>0.50550589701212278</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -1744,7 +1745,7 @@
       </c>
       <c r="F46">
         <f t="shared" si="0"/>
-        <v>293510</v>
+        <v>264206</v>
       </c>
       <c r="G46">
         <f t="shared" si="1"/>
@@ -1752,7 +1753,7 @@
       </c>
       <c r="H46">
         <f t="shared" si="2"/>
-        <v>0.46609160174425068</v>
+        <v>0.41955707720500662</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -1773,7 +1774,7 @@
       </c>
       <c r="F47">
         <f t="shared" si="0"/>
-        <v>333946</v>
+        <v>357846</v>
       </c>
       <c r="G47">
         <f t="shared" si="1"/>
@@ -1781,7 +1782,7 @@
       </c>
       <c r="H47">
         <f t="shared" si="2"/>
-        <v>0.46620318018734908</v>
+        <v>0.49956862252376766</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -1802,7 +1803,7 @@
       </c>
       <c r="F48">
         <f t="shared" si="0"/>
-        <v>406035</v>
+        <v>373841</v>
       </c>
       <c r="G48">
         <f t="shared" si="1"/>
@@ -1810,7 +1811,7 @@
       </c>
       <c r="H48">
         <f t="shared" si="2"/>
-        <v>0.52369448801023566</v>
+        <v>0.48217141648437822</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
@@ -1831,7 +1832,7 @@
       </c>
       <c r="F49">
         <f t="shared" si="0"/>
-        <v>76549</v>
+        <v>200377</v>
       </c>
       <c r="G49">
         <f t="shared" si="1"/>
@@ -1839,7 +1840,7 @@
       </c>
       <c r="H49">
         <f t="shared" si="2"/>
-        <v>9.0358914309592211E-2</v>
+        <v>0.23652625341432493</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -1860,7 +1861,7 @@
       </c>
       <c r="F50">
         <f t="shared" si="0"/>
-        <v>773409</v>
+        <v>715467</v>
       </c>
       <c r="G50">
         <f t="shared" si="1"/>
@@ -1868,7 +1869,7 @@
       </c>
       <c r="H50">
         <f t="shared" si="2"/>
-        <v>0.8553535840601284</v>
+        <v>0.79127248677833839</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -1889,7 +1890,7 @@
       </c>
       <c r="F51">
         <f t="shared" si="0"/>
-        <v>942663</v>
+        <v>976859</v>
       </c>
       <c r="G51">
         <f t="shared" si="1"/>
@@ -1897,7 +1898,7 @@
       </c>
       <c r="H51">
         <f t="shared" si="2"/>
-        <v>0.94946687965964094</v>
+        <v>0.98390969688789864</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -1918,7 +1919,7 @@
       </c>
       <c r="F52">
         <f t="shared" si="0"/>
-        <v>1638800</v>
+        <v>1328034</v>
       </c>
       <c r="G52">
         <f t="shared" si="1"/>
@@ -1926,7 +1927,7 @@
       </c>
       <c r="H52">
         <f t="shared" si="2"/>
-        <v>1.4931356577705375</v>
+        <v>1.2099920186304844</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -1947,7 +1948,7 @@
       </c>
       <c r="F53">
         <f t="shared" si="0"/>
-        <v>485522</v>
+        <v>251782</v>
       </c>
       <c r="G53">
         <f t="shared" si="1"/>
@@ -1955,7 +1956,7 @@
       </c>
       <c r="H53">
         <f t="shared" si="2"/>
-        <v>0.45746520171369726</v>
+        <v>0.23723230547303339</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -1976,7 +1977,7 @@
       </c>
       <c r="F54">
         <f t="shared" si="0"/>
-        <v>556783</v>
+        <v>196607</v>
       </c>
       <c r="G54">
         <f t="shared" si="1"/>
@@ -1984,7 +1985,7 @@
       </c>
       <c r="H54">
         <f t="shared" si="2"/>
-        <v>0.58482230543403479</v>
+        <v>0.2065080273723682</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -2005,7 +2006,7 @@
       </c>
       <c r="F55">
         <f t="shared" si="0"/>
-        <v>-168778</v>
+        <v>5284</v>
       </c>
       <c r="G55">
         <f t="shared" si="1"/>
@@ -2013,7 +2014,7 @@
       </c>
       <c r="H55">
         <f t="shared" si="2"/>
-        <v>-0.17282982235529759</v>
+        <v>5.4108520146310098E-3</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -2034,7 +2035,7 @@
       </c>
       <c r="F56">
         <f t="shared" si="0"/>
-        <v>969843</v>
+        <v>453627</v>
       </c>
       <c r="G56">
         <f t="shared" si="1"/>
@@ -2042,7 +2043,7 @@
       </c>
       <c r="H56">
         <f t="shared" si="2"/>
-        <v>0.9468543238707422</v>
+        <v>0.44287445119933144</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -2063,7 +2064,7 @@
       </c>
       <c r="F57">
         <f t="shared" si="0"/>
-        <v>1229662</v>
+        <v>625412</v>
       </c>
       <c r="G57">
         <f t="shared" si="1"/>
@@ -2071,7 +2072,7 @@
       </c>
       <c r="H57">
         <f t="shared" si="2"/>
-        <v>1.0657635521349298</v>
+        <v>0.54205246211382541</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -2092,7 +2093,7 @@
       </c>
       <c r="F58">
         <f t="shared" si="0"/>
-        <v>947213</v>
+        <v>288317</v>
       </c>
       <c r="G58">
         <f t="shared" si="1"/>
@@ -2100,7 +2101,7 @@
       </c>
       <c r="H58">
         <f t="shared" si="2"/>
-        <v>0.7376031497215727</v>
+        <v>0.22451500065800897</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -2121,7 +2122,7 @@
       </c>
       <c r="F59">
         <f t="shared" si="0"/>
-        <v>1381511</v>
+        <v>717427</v>
       </c>
       <c r="G59">
         <f t="shared" si="1"/>
@@ -2129,7 +2130,7 @@
       </c>
       <c r="H59">
         <f t="shared" si="2"/>
-        <v>0.99115038533668709</v>
+        <v>0.51471037689960009</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -2150,7 +2151,7 @@
       </c>
       <c r="F60">
         <f t="shared" si="0"/>
-        <v>-985228</v>
+        <v>318748</v>
       </c>
       <c r="G60">
         <f t="shared" si="1"/>
@@ -2158,7 +2159,7 @@
       </c>
       <c r="H60">
         <f t="shared" si="2"/>
-        <v>-0.69258953075088858</v>
+        <v>0.22407151212489315</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
@@ -2179,7 +2180,7 @@
       </c>
       <c r="F61">
         <f t="shared" si="0"/>
-        <v>710547</v>
+        <v>-295007</v>
       </c>
       <c r="G61">
         <f t="shared" si="1"/>
@@ -2187,7 +2188,7 @@
       </c>
       <c r="H61">
         <f t="shared" si="2"/>
-        <v>0.59173392805391123</v>
+        <v>-0.24567783821956915</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -2208,7 +2209,7 @@
       </c>
       <c r="F62">
         <f t="shared" si="0"/>
-        <v>862341</v>
+        <v>248159</v>
       </c>
       <c r="G62">
         <f t="shared" si="1"/>
@@ -2216,7 +2217,7 @@
       </c>
       <c r="H62">
         <f t="shared" si="2"/>
-        <v>0.69150974186093317</v>
+        <v>0.19899826870167059</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -2237,7 +2238,7 @@
       </c>
       <c r="F63">
         <f t="shared" si="0"/>
-        <v>351281</v>
+        <v>385949</v>
       </c>
       <c r="G63">
         <f t="shared" si="1"/>
@@ -2245,7 +2246,7 @@
       </c>
       <c r="H63">
         <f t="shared" si="2"/>
-        <v>0.2537200564526963</v>
+        <v>0.27875974524059566</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -2266,7 +2267,7 @@
       </c>
       <c r="F64">
         <f t="shared" si="0"/>
-        <v>-84116</v>
+        <v>698450</v>
       </c>
       <c r="G64">
         <f t="shared" si="1"/>
@@ -2274,7 +2275,7 @@
       </c>
       <c r="H64">
         <f t="shared" si="2"/>
-        <v>-5.4708632758969436E-2</v>
+        <v>0.45426844536713828</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
@@ -2295,7 +2296,7 @@
       </c>
       <c r="F65">
         <f t="shared" si="0"/>
-        <v>762934</v>
+        <v>652888</v>
       </c>
       <c r="G65">
         <f t="shared" si="1"/>
@@ -2303,7 +2304,7 @@
       </c>
       <c r="H65">
         <f t="shared" si="2"/>
-        <v>0.47937413329764422</v>
+        <v>0.41022895707942275</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -2324,7 +2325,7 @@
       </c>
       <c r="F66">
         <f t="shared" si="0"/>
-        <v>362433</v>
+        <v>984745</v>
       </c>
       <c r="G66">
         <f t="shared" si="1"/>
@@ -2332,7 +2333,7 @@
       </c>
       <c r="H66">
         <f t="shared" si="2"/>
-        <v>0.20757630340493796</v>
+        <v>0.56399314327474492</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -2352,8 +2353,8 @@
         <v>-86489</v>
       </c>
       <c r="F67">
-        <f t="shared" ref="F67:F71" si="3">D67+E67</f>
-        <v>1053482</v>
+        <f t="shared" ref="F67:F71" si="3">D67-E67</f>
+        <v>1226460</v>
       </c>
       <c r="G67">
         <f t="shared" ref="G67:G71" si="4">B67/C67</f>
@@ -2361,7 +2362,7 @@
       </c>
       <c r="H67">
         <f t="shared" ref="H67:H71" si="5">F67/C67</f>
-        <v>0.58869298982356788</v>
+        <v>0.68535428635611528</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -2382,7 +2383,7 @@
       </c>
       <c r="F68">
         <f t="shared" si="3"/>
-        <v>1027623</v>
+        <v>876025</v>
       </c>
       <c r="G68">
         <f t="shared" si="4"/>
@@ -2390,7 +2391,7 @@
       </c>
       <c r="H68">
         <f t="shared" si="5"/>
-        <v>0.58582290142308002</v>
+        <v>0.49940056540107963</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -2411,7 +2412,7 @@
       </c>
       <c r="F69">
         <f t="shared" si="3"/>
-        <v>622581</v>
+        <v>472905</v>
       </c>
       <c r="G69">
         <f t="shared" si="4"/>
@@ -2419,7 +2420,7 @@
       </c>
       <c r="H69">
         <f t="shared" si="5"/>
-        <v>0.333644873335945</v>
+        <v>0.25343261170022063</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -2440,7 +2441,7 @@
       </c>
       <c r="F70">
         <f t="shared" si="3"/>
-        <v>754798</v>
+        <v>986156</v>
       </c>
       <c r="G70">
         <f t="shared" si="4"/>
@@ -2448,7 +2449,7 @@
       </c>
       <c r="H70">
         <f t="shared" si="5"/>
-        <v>0.37422556719022687</v>
+        <v>0.48893185784547039</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
@@ -2469,7 +2470,7 @@
       </c>
       <c r="F71">
         <f t="shared" si="3"/>
-        <v>241018</v>
+        <v>1261712</v>
       </c>
       <c r="G71">
         <f t="shared" si="4"/>
@@ -2477,7 +2478,7 @@
       </c>
       <c r="H71">
         <f t="shared" si="5"/>
-        <v>0.114905407969549</v>
+        <v>0.60152159631262236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>